<commit_message>
Added creature and item models
</commit_message>
<xml_diff>
--- a/venv/data_model/realms_model.xlsx
+++ b/venv/data_model/realms_model.xlsx
@@ -206,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -216,10 +216,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -349,10 +345,13 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.95"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -387,7 +386,7 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2" t="n">
@@ -405,7 +404,7 @@
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2"/>
@@ -420,7 +419,7 @@
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2"/>
@@ -435,7 +434,7 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -449,7 +448,7 @@
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -463,7 +462,7 @@
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -477,7 +476,7 @@
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="n">
@@ -495,7 +494,7 @@
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="2" t="n">
@@ -516,7 +515,7 @@
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -530,7 +529,7 @@
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -544,7 +543,7 @@
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -558,7 +557,7 @@
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -572,7 +571,7 @@
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -586,7 +585,7 @@
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -600,10 +599,11 @@
       <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="3" t="b">
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -614,10 +614,10 @@
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -628,16 +628,17 @@
       <c r="B18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="3" t="b">
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -648,10 +649,10 @@
       <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -662,10 +663,10 @@
       <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -676,10 +677,10 @@
       <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -690,10 +691,10 @@
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -704,10 +705,10 @@
       <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>